<commit_message>
Improve Excek reading... again
</commit_message>
<xml_diff>
--- a/scautable/test/resources/Numbers.xlsx
+++ b/scautable/test/resources/Numbers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\scautable\scautable\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F0F29BE-434F-48FC-8685-AD9534ECBCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C59852B-74A4-43CB-8E60-582E8FEBBF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="29010" windowHeight="23385" xr2:uid="{54CAD6A3-1767-48FD-929F-C35C3613C9E6}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="43200" windowHeight="17145" xr2:uid="{54CAD6A3-1767-48FD-929F-C35C3613C9E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +426,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,13 +446,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -459,13 +460,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>3</v>
       </c>
       <c r="D3" t="s">

</xml_diff>